<commit_message>
agregado PabloSanMartin, actualizado gitignore
</commit_message>
<xml_diff>
--- a/filesystem/pdmtktr/correctivos/constantes/coordinadoresTorresRegiones.xlsx
+++ b/filesystem/pdmtktr/correctivos/constantes/coordinadoresTorresRegiones.xlsx
@@ -40,10 +40,10 @@
     <t xml:space="preserve">COMUNICACIONES</t>
   </si>
   <si>
-    <t xml:space="preserve">MARTIN PALMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YP11856</t>
+    <t xml:space="preserve">PABLO SEBASTIAN SAN MARTIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE45933</t>
   </si>
   <si>
     <t xml:space="preserve">INFRAESTRUCTURA</t>
@@ -116,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,12 +138,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,12 +182,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,196 +387,196 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:D13"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PABLO SAN MARTIN (TEMPLATES TAMBIEN)
</commit_message>
<xml_diff>
--- a/filesystem/pdmtktr/correctivos/constantes/coordinadoresTorresRegiones.xlsx
+++ b/filesystem/pdmtktr/correctivos/constantes/coordinadoresTorresRegiones.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">COMUNICACIONES</t>
   </si>
   <si>
-    <t xml:space="preserve">PABLO SEBASTIAN SAN MARTIN</t>
+    <t xml:space="preserve">PABLO MIGUEL SAN MARTIN</t>
   </si>
   <si>
     <t xml:space="preserve">SE45933</t>
@@ -387,7 +387,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>